<commit_message>
Added docuemnt request and word and update
</commit_message>
<xml_diff>
--- a/employeesDB.xlsx
+++ b/employeesDB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -32,9 +32,6 @@
     <t>javier</t>
   </si>
   <si>
-    <t>22da</t>
-  </si>
-  <si>
     <t>tatis</t>
   </si>
   <si>
@@ -42,6 +39,12 @@
   </si>
   <si>
     <t>maldonado</t>
+  </si>
+  <si>
+    <t>Amarilis</t>
+  </si>
+  <si>
+    <t>marca</t>
   </si>
 </sst>
 </file>
@@ -138,44 +141,44 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s" s="2">
         <v>6</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>2341.0</v>
+        <v>12322.0</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>2341.0</v>
+        <v>12322.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>12322.0</v>
+        <v>12212.0</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>12322.0</v>
+        <v>12212.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>12212.0</v>
+        <v>12321.0</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>12212.0</v>
+        <v>12321.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>